<commit_message>
1. Clean up 2. import 1/10 build case 3. import dumpSite
</commit_message>
<xml_diff>
--- a/import/buildCase1.xlsx
+++ b/import/buildCase1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="30" windowWidth="15600" windowHeight="2280" firstSheet="2" activeTab="8"/>
+    <workbookView xWindow="-15" yWindow="30" windowWidth="15600" windowHeight="2280"/>
   </bookViews>
   <sheets>
     <sheet name="基隆已發建照" sheetId="13" r:id="rId1"/>
@@ -6131,7 +6131,7 @@
   </sheetPr>
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B86" sqref="B86"/>
       <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
@@ -16734,7 +16734,7 @@
   </sheetPr>
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B86" sqref="B86"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>

</xml_diff>